<commit_message>
Got rid of redundant policy lines
</commit_message>
<xml_diff>
--- a/results/02-2023/comparison-deflators-02-2023.xlsx
+++ b/results/02-2023/comparison-deflators-02-2023.xlsx
@@ -743,31 +743,31 @@
         <v>-0.9599</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.3966</v>
+        <v>-0.4662</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0496</v>
+        <v>-0.0489</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.0516</v>
+        <v>-0.0509</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.0276</v>
+        <v>-0.0429</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.296</v>
+        <v>-0.295</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.4283</v>
+        <v>-0.4274</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.0622</v>
+        <v>-0.0613</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.0142</v>
+        <v>-0.0499</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.3911</v>
+        <v>-0.3899</v>
       </c>
     </row>
     <row r="6">
@@ -799,31 +799,31 @@
         <v>-0.034</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.1007</v>
+        <v>-0.0641</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.1058</v>
+        <v>-0.0694</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0889</v>
+        <v>-0.0526</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.083</v>
+        <v>-0.0471</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0704</v>
+        <v>-0.0352</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.0546</v>
+        <v>-0.0202</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.0561</v>
+        <v>-0.0223</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.0372</v>
+        <v>-0.0112</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.0356</v>
+        <v>-0.0101</v>
       </c>
     </row>
     <row r="7">
@@ -855,31 +855,31 @@
         <v>-0.0589</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0966</v>
+        <v>-0.1115</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0657</v>
+        <v>-0.0957</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.0972</v>
+        <v>-0.1426</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.1045</v>
+        <v>-0.1501</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.107</v>
+        <v>-0.1383</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0211</v>
+        <v>-0.038</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0176</v>
+        <v>0.0151</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0223</v>
+        <v>0.0197</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0327</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8">
@@ -911,31 +911,31 @@
         <v>-0.4134</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.1178</v>
+        <v>-0.117</v>
       </c>
       <c r="K8" t="n">
-        <v>0.055</v>
+        <v>0.0557</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1073</v>
+        <v>0.1076</v>
       </c>
       <c r="M8" t="n">
-        <v>0.179</v>
+        <v>0.1645</v>
       </c>
       <c r="N8" t="n">
-        <v>0.4505</v>
+        <v>0.4363</v>
       </c>
       <c r="O8" t="n">
-        <v>0.4366</v>
+        <v>0.4298</v>
       </c>
       <c r="P8" t="n">
-        <v>0.4479</v>
+        <v>0.4413</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4021</v>
+        <v>0.4039</v>
       </c>
       <c r="R8" t="n">
-        <v>0.2878</v>
+        <v>0.2893</v>
       </c>
     </row>
     <row r="9">
@@ -1359,31 +1359,31 @@
         <v>-1.0237</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.4993</v>
+        <v>-1.5464</v>
       </c>
       <c r="K16" t="n">
-        <v>-1.6586</v>
+        <v>-1.6509</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.5768</v>
+        <v>-0.585</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.5236</v>
+        <v>-0.5631</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.6023</v>
+        <v>-0.6118</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.2009</v>
+        <v>-0.1892</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.1591</v>
+        <v>-0.1336</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0349</v>
+        <v>0.0243</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.0733</v>
+        <v>-0.0478</v>
       </c>
     </row>
     <row r="17">
@@ -2311,31 +2311,31 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>0.0003</v>
+        <v>-0.0693</v>
       </c>
       <c r="K33" t="n">
-        <v>0.0118</v>
+        <v>0.0125</v>
       </c>
       <c r="L33" t="n">
-        <v>0.1132</v>
+        <v>0.114</v>
       </c>
       <c r="M33" t="n">
-        <v>0.0962</v>
+        <v>0.081</v>
       </c>
       <c r="N33" t="n">
-        <v>0.0186</v>
+        <v>0.0196</v>
       </c>
       <c r="O33" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
       <c r="P33" t="n">
-        <v>0.0227</v>
+        <v>0.0236</v>
       </c>
       <c r="Q33" t="n">
-        <v>0.0113</v>
+        <v>-0.0244</v>
       </c>
       <c r="R33" t="n">
-        <v>0.0344</v>
+        <v>0.0356</v>
       </c>
     </row>
     <row r="34">
@@ -2367,31 +2367,31 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0.0035</v>
+        <v>0.04</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0049</v>
+        <v>0.0413</v>
       </c>
       <c r="L34" t="n">
-        <v>0.0067</v>
+        <v>0.0429</v>
       </c>
       <c r="M34" t="n">
-        <v>0.0089</v>
+        <v>0.0448</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0112</v>
+        <v>0.0464</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0136</v>
+        <v>0.0481</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0157</v>
+        <v>0.0495</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.0153</v>
+        <v>0.0412</v>
       </c>
       <c r="R34" t="n">
-        <v>0.0109</v>
+        <v>0.0365</v>
       </c>
     </row>
     <row r="35">
@@ -2423,31 +2423,31 @@
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.0303</v>
+        <v>-0.0452</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.0578</v>
+        <v>-0.0879</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.0846</v>
+        <v>-0.1301</v>
       </c>
       <c r="M35" t="n">
-        <v>-0.0862</v>
+        <v>-0.1319</v>
       </c>
       <c r="N35" t="n">
-        <v>-0.0553</v>
+        <v>-0.0867</v>
       </c>
       <c r="O35" t="n">
-        <v>-0.0244</v>
+        <v>-0.0414</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0051</v>
+        <v>0.0026</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.0102</v>
+        <v>0.0076</v>
       </c>
       <c r="R35" t="n">
-        <v>0.0114</v>
+        <v>0.0087</v>
       </c>
     </row>
     <row r="36">
@@ -2479,31 +2479,31 @@
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>0.0672</v>
+        <v>0.0679</v>
       </c>
       <c r="K36" t="n">
-        <v>0.1296</v>
+        <v>0.1303</v>
       </c>
       <c r="L36" t="n">
-        <v>0.1574</v>
+        <v>0.1576</v>
       </c>
       <c r="M36" t="n">
-        <v>0.1329</v>
+        <v>0.1184</v>
       </c>
       <c r="N36" t="n">
-        <v>0.1065</v>
+        <v>0.0922</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0991</v>
+        <v>0.0924</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0935</v>
+        <v>0.0869</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.0592</v>
+        <v>0.061</v>
       </c>
       <c r="R36" t="n">
-        <v>-0.0041</v>
+        <v>-0.0027</v>
       </c>
     </row>
     <row r="37">
@@ -2927,31 +2927,31 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.0275</v>
+        <v>-0.0746</v>
       </c>
       <c r="K44" t="n">
-        <v>0.1313</v>
+        <v>0.1391</v>
       </c>
       <c r="L44" t="n">
-        <v>0.3068</v>
+        <v>0.2986</v>
       </c>
       <c r="M44" t="n">
-        <v>0.1793</v>
+        <v>0.1398</v>
       </c>
       <c r="N44" t="n">
-        <v>0.1402</v>
+        <v>0.1308</v>
       </c>
       <c r="O44" t="n">
-        <v>0.1432</v>
+        <v>0.1549</v>
       </c>
       <c r="P44" t="n">
-        <v>0.1766</v>
+        <v>0.2022</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.1286</v>
+        <v>0.1181</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.1075</v>
+        <v>-0.082</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
Full CBO changes after talking to Louise
</commit_message>
<xml_diff>
--- a/results/02-2023/comparison-deflators-02-2023.xlsx
+++ b/results/02-2023/comparison-deflators-02-2023.xlsx
@@ -823,7 +823,7 @@
         <v>-0.0112</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.0101</v>
+        <v>-0.0154</v>
       </c>
     </row>
     <row r="7">
@@ -1123,43 +1123,43 @@
         <v>0.2068</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.9264</v>
+        <v>-0.9172</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.2423</v>
+        <v>-0.2334</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.8494</v>
+        <v>-0.8409</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.4288</v>
+        <v>-0.4083</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0029</v>
+        <v>0.0142</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1128</v>
+        <v>0.124</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1612</v>
+        <v>0.1722</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.1005</v>
+        <v>-0.1072</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.1037</v>
+        <v>-0.1102</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0886</v>
+        <v>-0.095</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0738</v>
+        <v>-0.08</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0456</v>
+        <v>-0.0445</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0806</v>
+        <v>-0.0796</v>
       </c>
     </row>
     <row r="13">
@@ -1347,43 +1347,43 @@
         <v>-3.0855</v>
       </c>
       <c r="F16" t="n">
-        <v>-3.8432</v>
+        <v>-3.8339</v>
       </c>
       <c r="G16" t="n">
-        <v>-4.8306</v>
+        <v>-4.8217</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.486</v>
+        <v>-2.4774</v>
       </c>
       <c r="I16" t="n">
-        <v>-1.0237</v>
+        <v>-1.0032</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.5464</v>
+        <v>-1.5351</v>
       </c>
       <c r="K16" t="n">
-        <v>-1.6509</v>
+        <v>-1.6397</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.585</v>
+        <v>-0.574</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.5631</v>
+        <v>-0.5699</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.6118</v>
+        <v>-0.6183</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.1892</v>
+        <v>-0.1956</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.1336</v>
+        <v>-0.1398</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0243</v>
+        <v>0.0254</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.0478</v>
+        <v>-0.052</v>
       </c>
     </row>
     <row r="17">
@@ -2391,7 +2391,7 @@
         <v>0.0412</v>
       </c>
       <c r="R34" t="n">
-        <v>0.0365</v>
+        <v>0.0312</v>
       </c>
     </row>
     <row r="35">
@@ -2691,43 +2691,43 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>0.0092</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>0.0089</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>0.0086</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>0.0205</v>
       </c>
       <c r="J40" t="n">
-        <v>-0.0151</v>
+        <v>-0.0038</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.0273</v>
+        <v>-0.0161</v>
       </c>
       <c r="L40" t="n">
-        <v>-0.0384</v>
+        <v>-0.0274</v>
       </c>
       <c r="M40" t="n">
-        <v>-0.049</v>
+        <v>-0.0558</v>
       </c>
       <c r="N40" t="n">
-        <v>-0.0373</v>
+        <v>-0.0439</v>
       </c>
       <c r="O40" t="n">
-        <v>-0.0248</v>
+        <v>-0.0312</v>
       </c>
       <c r="P40" t="n">
-        <v>-0.0122</v>
+        <v>-0.0184</v>
       </c>
       <c r="Q40" t="n">
-        <v>-0.0047</v>
+        <v>-0.0036</v>
       </c>
       <c r="R40" t="n">
-        <v>-0.0023</v>
+        <v>-0.0013</v>
       </c>
     </row>
     <row r="41">
@@ -2915,43 +2915,43 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>0.0092</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>0.0089</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>0.0086</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>0.0205</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.0746</v>
+        <v>-0.0632</v>
       </c>
       <c r="K44" t="n">
-        <v>0.1391</v>
+        <v>0.1503</v>
       </c>
       <c r="L44" t="n">
-        <v>0.2986</v>
+        <v>0.3096</v>
       </c>
       <c r="M44" t="n">
-        <v>0.1398</v>
+        <v>0.1331</v>
       </c>
       <c r="N44" t="n">
-        <v>0.1308</v>
+        <v>0.1242</v>
       </c>
       <c r="O44" t="n">
-        <v>0.1549</v>
+        <v>0.1485</v>
       </c>
       <c r="P44" t="n">
-        <v>0.2022</v>
+        <v>0.196</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.1181</v>
+        <v>0.1191</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.082</v>
+        <v>-0.0862</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
ran fim, pulled in mpi, edited social benefits sheet
u
</commit_message>
<xml_diff>
--- a/results/02-2023/comparison-deflators-02-2023.xlsx
+++ b/results/02-2023/comparison-deflators-02-2023.xlsx
@@ -1135,31 +1135,31 @@
         <v>-0.4</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0215</v>
+        <v>0.0191</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1293</v>
+        <v>0.1269</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1754</v>
+        <v>0.1731</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.1079</v>
+        <v>-0.1102</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.1106</v>
+        <v>-0.0957</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0954</v>
+        <v>-0.0808</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0803</v>
+        <v>-0.066</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0448</v>
+        <v>-0.0309</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0799</v>
+        <v>-0.0692</v>
       </c>
     </row>
     <row r="13">
@@ -1359,31 +1359,31 @@
         <v>-1.0297</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.4846</v>
+        <v>-1.488</v>
       </c>
       <c r="K16" t="n">
-        <v>-1.604</v>
+        <v>-1.6061</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.5373</v>
+        <v>-0.5396</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.5602</v>
+        <v>-0.5624</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.612</v>
+        <v>-0.5968</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.1923</v>
+        <v>-0.1776</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.1197</v>
+        <v>-0.1055</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0289</v>
+        <v>0.0429</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.1199</v>
+        <v>0.0089</v>
       </c>
     </row>
     <row r="17">
@@ -1719,7 +1719,7 @@
         <v>-0.1013</v>
       </c>
       <c r="R22" t="n">
-        <v>0.1097</v>
+        <v>0.2276</v>
       </c>
     </row>
     <row r="23">
@@ -2087,31 +2087,31 @@
         <v>-0.0473</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.0265</v>
+        <v>-0.0275</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.0064</v>
+        <v>-0.0062</v>
       </c>
       <c r="L29" t="n">
-        <v>0.007</v>
+        <v>0.0071</v>
       </c>
       <c r="M29" t="n">
         <v>0.016</v>
       </c>
       <c r="N29" t="n">
-        <v>0.0119</v>
+        <v>0.0122</v>
       </c>
       <c r="O29" t="n">
-        <v>0.0073</v>
+        <v>0.0075</v>
       </c>
       <c r="P29" t="n">
         <v>0.0025</v>
       </c>
       <c r="Q29" t="n">
-        <v>-0.0017</v>
+        <v>-0.0016</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.0042</v>
+        <v>-0.004</v>
       </c>
     </row>
     <row r="30">
@@ -2703,31 +2703,31 @@
         <v>0.0083</v>
       </c>
       <c r="J40" t="n">
-        <v>0.0073</v>
+        <v>0.0049</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0053</v>
+        <v>0.003</v>
       </c>
       <c r="L40" t="n">
-        <v>0.0032</v>
+        <v>0.0009</v>
       </c>
       <c r="M40" t="n">
-        <v>-0.0007</v>
+        <v>-0.003</v>
       </c>
       <c r="N40" t="n">
-        <v>-0.0004</v>
+        <v>0.0145</v>
       </c>
       <c r="O40" t="n">
-        <v>-0.0003</v>
+        <v>0.0142</v>
       </c>
       <c r="P40" t="n">
-        <v>-0.0003</v>
+        <v>0.0139</v>
       </c>
       <c r="Q40" t="n">
-        <v>-0.0003</v>
+        <v>0.0136</v>
       </c>
       <c r="R40" t="n">
-        <v>-0.0003</v>
+        <v>0.0105</v>
       </c>
     </row>
     <row r="41">
@@ -2927,31 +2927,31 @@
         <v>-0.0265</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0505</v>
+        <v>0.0471</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0357</v>
+        <v>0.0335</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0367</v>
+        <v>0.0344</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0097</v>
+        <v>0.0075</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0063</v>
+        <v>0.0215</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0032</v>
+        <v>0.018</v>
       </c>
       <c r="P44" t="n">
-        <v>0.0201</v>
+        <v>0.0343</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.0035</v>
+        <v>0.0175</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.0679</v>
+        <v>0.0609</v>
       </c>
     </row>
     <row r="45">
@@ -3287,7 +3287,7 @@
         <v>-0.0001</v>
       </c>
       <c r="R50" t="n">
-        <v>-0.0716</v>
+        <v>0.0463</v>
       </c>
     </row>
     <row r="51">
@@ -3655,22 +3655,22 @@
         <v>0</v>
       </c>
       <c r="J57" t="n">
+        <v>-0.0007</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="L57" t="n">
         <v>0.0004</v>
       </c>
-      <c r="K57" t="n">
+      <c r="M57" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="O57" t="n">
         <v>0.0003</v>
-      </c>
-      <c r="L57" t="n">
-        <v>0.0003</v>
-      </c>
-      <c r="M57" t="n">
-        <v>0.0003</v>
-      </c>
-      <c r="N57" t="n">
-        <v>0.0002</v>
-      </c>
-      <c r="O57" t="n">
-        <v>0.0001</v>
       </c>
       <c r="P57" t="n">
         <v>0.0001</v>
@@ -3679,7 +3679,7 @@
         <v>0.0001</v>
       </c>
       <c r="R57" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="58">

</xml_diff>